<commit_message>
Revert FileAnnotationTemplate.xlsx to commit 922b895
</commit_message>
<xml_diff>
--- a/current-excel-manifests/FileAnnotationTemplate.xlsx
+++ b/current-excel-manifests/FileAnnotationTemplate.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="565">
   <si>
     <t>Component</t>
   </si>
@@ -984,7 +984,7 @@
     <t>json</t>
   </si>
   <si>
-    <t>DivCo_HS</t>
+    <t>DukeAD_PTSD</t>
   </si>
   <si>
     <t>transcript quantification</t>
@@ -996,7 +996,7 @@
     <t>locs</t>
   </si>
   <si>
-    <t>DukeAD_PTSD</t>
+    <t>ELPSCRNA</t>
   </si>
   <si>
     <t>variancePartition</t>
@@ -1008,7 +1008,7 @@
     <t>maf</t>
   </si>
   <si>
-    <t>ELPSCRNA</t>
+    <t>Emory_ADRC</t>
   </si>
   <si>
     <t>Variant calling</t>
@@ -1020,7 +1020,7 @@
     <t>mat</t>
   </si>
   <si>
-    <t>Emory_ADRC</t>
+    <t>Emory_Levey_300_CSF_FNIH</t>
   </si>
   <si>
     <t>visualization</t>
@@ -1032,7 +1032,7 @@
     <t>md</t>
   </si>
   <si>
-    <t>Emory_Levey_300_CSF_FNIH</t>
+    <t>EmoryDrosophilaTau</t>
   </si>
   <si>
     <t>LC-SRM</t>
@@ -1041,7 +1041,7 @@
     <t>mov</t>
   </si>
   <si>
-    <t>EmoryDrosophilaTau</t>
+    <t>EpiGABA</t>
   </si>
   <si>
     <t>Leiden Oxylipins</t>
@@ -1050,7 +1050,7 @@
     <t>mp4</t>
   </si>
   <si>
-    <t>EpiGABA</t>
+    <t>EpiMap</t>
   </si>
   <si>
     <t>lentiMPRA</t>
@@ -1059,7 +1059,7 @@
     <t>msf</t>
   </si>
   <si>
-    <t>EpiMap</t>
+    <t>eQTLmetaAnalysis</t>
   </si>
   <si>
     <t>LFP</t>
@@ -1068,7 +1068,7 @@
     <t>mtx</t>
   </si>
   <si>
-    <t>eQTLmetaAnalysis</t>
+    <t>FreshMicro</t>
   </si>
   <si>
     <t>liquid chromatography-electrochemical detection</t>
@@ -1077,7 +1077,7 @@
     <t>nirs</t>
   </si>
   <si>
-    <t>FreshMicro</t>
+    <t>HBI_scRNAseq</t>
   </si>
   <si>
     <t>lncrnaSeq</t>
@@ -1086,7 +1086,7 @@
     <t>pdf</t>
   </si>
   <si>
-    <t>HBI_scRNAseq</t>
+    <t>HBTRC</t>
   </si>
   <si>
     <t>locomotor activation behavior</t>
@@ -1095,7 +1095,7 @@
     <t>pdresult</t>
   </si>
   <si>
-    <t>HBTRC</t>
+    <t>HDAC1-cKOBrain</t>
   </si>
   <si>
     <t>long-read rnaSeq</t>
@@ -1104,7 +1104,7 @@
     <t>pdstudy</t>
   </si>
   <si>
-    <t>HDAC1-cKOBrain</t>
+    <t>HumanFC</t>
   </si>
   <si>
     <t>LTP</t>
@@ -1113,7 +1113,7 @@
     <t>pdview</t>
   </si>
   <si>
-    <t>HumanFC</t>
+    <t>IL10_APPmouse</t>
   </si>
   <si>
     <t>m6A-rnaSeq</t>
@@ -1122,7 +1122,7 @@
     <t>plink</t>
   </si>
   <si>
-    <t>IL10_APPmouse</t>
+    <t>iNiAstshRNA</t>
   </si>
   <si>
     <t>MDMS-SL</t>
@@ -1131,7 +1131,7 @@
     <t>png</t>
   </si>
   <si>
-    <t>iNiAstshRNA</t>
+    <t>IntegrativePathwayAnalysis</t>
   </si>
   <si>
     <t>memory behavior</t>
@@ -1140,7 +1140,7 @@
     <t>powerpoint</t>
   </si>
   <si>
-    <t>IntegrativePathwayAnalysis</t>
+    <t>iPSC</t>
   </si>
   <si>
     <t>Metabolon</t>
@@ -1149,7 +1149,7 @@
     <t>Python script</t>
   </si>
   <si>
-    <t>iPSC</t>
+    <t>iPSC-HiC</t>
   </si>
   <si>
     <t>methylationArray</t>
@@ -1158,7 +1158,7 @@
     <t>pzfx</t>
   </si>
   <si>
-    <t>iPSC-HiC</t>
+    <t>iPSCAstrocytes</t>
   </si>
   <si>
     <t>MIB/MS</t>
@@ -1167,13 +1167,13 @@
     <t>R script</t>
   </si>
   <si>
-    <t>iPSCAstrocytes</t>
+    <t>iPSCMicroglia</t>
   </si>
   <si>
     <t>microRNAcounts</t>
   </si>
   <si>
-    <t>iPSCMicroglia</t>
+    <t>ISB_Taner_CollagenDomain</t>
   </si>
   <si>
     <t>mirnaArray</t>
@@ -1182,7 +1182,7 @@
     <t>RCC</t>
   </si>
   <si>
-    <t>ISB_Taner_CollagenDomain</t>
+    <t>ISB_Taner_Cxcl10</t>
   </si>
   <si>
     <t>mirnaSeq</t>
@@ -1191,7 +1191,7 @@
     <t>RData</t>
   </si>
   <si>
-    <t>ISB_Taner_Cxcl10</t>
+    <t>ISB_Taner_PTN_MDK</t>
   </si>
   <si>
     <t>MRI</t>
@@ -1200,7 +1200,7 @@
     <t>recal</t>
   </si>
   <si>
-    <t>ISB_Taner_PTN_MDK</t>
+    <t>ISB_Taner_sIL10r_sIL4r</t>
   </si>
   <si>
     <t>mRNAcounts</t>
@@ -1209,7 +1209,7 @@
     <t>RLF</t>
   </si>
   <si>
-    <t>ISB_Taner_sIL10r_sIL4r</t>
+    <t>ISB_Taner_TGFbeta</t>
   </si>
   <si>
     <t>mRNAseq</t>
@@ -1218,7 +1218,7 @@
     <t>rmd</t>
   </si>
   <si>
-    <t>ISB_Taner_TGFbeta</t>
+    <t>Jax.IU.Pitt.Proteomics_Metabolomics_Pilot</t>
   </si>
   <si>
     <t>MudPIT</t>
@@ -1227,7 +1227,7 @@
     <t>saf</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt.Proteomics_Metabolomics_Pilot</t>
+    <t>Jax.IU.Pitt_APOE4.Trem2.R47H</t>
   </si>
   <si>
     <t>nextGenerationTargetedSequencing</t>
@@ -1236,7 +1236,7 @@
     <t>sam</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_APOE4.Trem2.R47H</t>
+    <t>Jax.IU.Pitt_APP.PS1</t>
   </si>
   <si>
     <t>Nightingale NMR</t>
@@ -1245,7 +1245,7 @@
     <t>sav</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_APP.PS1</t>
+    <t>Jax.IU.Pitt_Levetiracetam-5XFAD</t>
   </si>
   <si>
     <t>NOMe-Seq</t>
@@ -1254,7 +1254,7 @@
     <t>sdf</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_Levetiracetam-5XFAD</t>
+    <t>Jax.IU.Pitt_LOAD2.PrimaryScreen</t>
   </si>
   <si>
     <t>novelty response behavior</t>
@@ -1263,7 +1263,7 @@
     <t>seg</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_LOAD2.PrimaryScreen</t>
+    <t>Jax.IU.Pitt_MicrobiomePilot</t>
   </si>
   <si>
     <t>open field test</t>
@@ -1272,7 +1272,7 @@
     <t>Sentrix descriptor file</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_MicrobiomePilot</t>
+    <t>Jax.IU.Pitt_PrimaryScreen</t>
   </si>
   <si>
     <t>oxBS-Seq</t>
@@ -1281,7 +1281,7 @@
     <t>sf3</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_PrimaryScreen</t>
+    <t>Jax.IU.Pitt_StrainValidation</t>
   </si>
   <si>
     <t>pharmacodynamics</t>
@@ -1290,7 +1290,7 @@
     <t>sif</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_StrainValidation</t>
+    <t>Jax.IU.Pitt_Verubecestat_5XFAD</t>
   </si>
   <si>
     <t>pharmacokinetics</t>
@@ -1299,7 +1299,7 @@
     <t>sqlite</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_Verubecestat_5XFAD</t>
+    <t>LBP</t>
   </si>
   <si>
     <t>photograph</t>
@@ -1308,7 +1308,7 @@
     <t>sra</t>
   </si>
   <si>
-    <t>LBP</t>
+    <t>LillyMicroglia</t>
   </si>
   <si>
     <t>polymeraseChainReaction</t>
@@ -1317,7 +1317,7 @@
     <t>svg</t>
   </si>
   <si>
-    <t>LillyMicroglia</t>
+    <t>LLFS</t>
   </si>
   <si>
     <t>Positron Emission Tomography</t>
@@ -1326,7 +1326,7 @@
     <t>svs</t>
   </si>
   <si>
-    <t>LLFS</t>
+    <t>lncRNA Pilot</t>
   </si>
   <si>
     <t>proximity extension assay</t>
@@ -1335,7 +1335,7 @@
     <t>Synapse Table</t>
   </si>
   <si>
-    <t>lncRNA Pilot</t>
+    <t>MARS WISCONSIN</t>
   </si>
   <si>
     <t>questionnaire</t>
@@ -1344,7 +1344,7 @@
     <t>tab</t>
   </si>
   <si>
-    <t>MARS WISCONSIN</t>
+    <t>MayoeGWAS</t>
   </si>
   <si>
     <t>Rader Lipidomics</t>
@@ -1353,7 +1353,7 @@
     <t>tagAlign</t>
   </si>
   <si>
-    <t>MayoeGWAS</t>
+    <t>MayoHippocampus</t>
   </si>
   <si>
     <t>Real Time PCR</t>
@@ -1362,7 +1362,7 @@
     <t>tar</t>
   </si>
   <si>
-    <t>MayoHippocampus</t>
+    <t>MayoLOADGWAS</t>
   </si>
   <si>
     <t>Ribo-Seq</t>
@@ -1371,7 +1371,7 @@
     <t>tbi</t>
   </si>
   <si>
-    <t>MayoLOADGWAS</t>
+    <t>MayoPilotRNAseq</t>
   </si>
   <si>
     <t>rnaArray</t>
@@ -1380,7 +1380,7 @@
     <t>tif</t>
   </si>
   <si>
-    <t>MayoPilotRNAseq</t>
+    <t>MayoRNAseq</t>
   </si>
   <si>
     <t>rnaSeq</t>
@@ -1389,7 +1389,7 @@
     <t>tranches</t>
   </si>
   <si>
-    <t>MayoRNAseq</t>
+    <t>MC-BrAD</t>
   </si>
   <si>
     <t>rotarod performance test</t>
@@ -1398,7 +1398,7 @@
     <t>tsv</t>
   </si>
   <si>
-    <t>MC-BrAD</t>
+    <t>MC-CAA</t>
   </si>
   <si>
     <t>RPPA</t>
@@ -1407,7 +1407,7 @@
     <t>txt</t>
   </si>
   <si>
-    <t>MC-CAA</t>
+    <t>MC_snRNA</t>
   </si>
   <si>
     <t>RRBS</t>
@@ -1416,7 +1416,7 @@
     <t>vcf</t>
   </si>
   <si>
-    <t>MC_snRNA</t>
+    <t>mCITE-Seq</t>
   </si>
   <si>
     <t>sandwich ELISA</t>
@@ -1425,7 +1425,7 @@
     <t>wiggle</t>
   </si>
   <si>
-    <t>mCITE-Seq</t>
+    <t>MCMPS</t>
   </si>
   <si>
     <t>Sanger sequencing</t>
@@ -1434,7 +1434,7 @@
     <t>xml</t>
   </si>
   <si>
-    <t>MCMPS</t>
+    <t>MEF2_Resilience</t>
   </si>
   <si>
     <t>scale</t>
@@ -1443,7 +1443,7 @@
     <t>yaml</t>
   </si>
   <si>
-    <t>MEF2_Resilience</t>
+    <t>MindPhenomeKB</t>
   </si>
   <si>
     <t>scATACSeq</t>
@@ -1452,165 +1452,162 @@
     <t>zip</t>
   </si>
   <si>
-    <t>MindPhenomeKB</t>
+    <t>miR155</t>
   </si>
   <si>
     <t>scCGIseq</t>
   </si>
   <si>
-    <t>miR155</t>
+    <t>MIT_ROSMAP_Multiomics</t>
   </si>
   <si>
     <t>scirnaSeq</t>
   </si>
   <si>
-    <t>MIT_ROSMAP_Multiomics</t>
+    <t>MOA-PAD</t>
   </si>
   <si>
     <t>scrnaSeq</t>
   </si>
   <si>
-    <t>MOA-PAD</t>
+    <t>MODEL-AD_5XFAD</t>
   </si>
   <si>
     <t>scwholeGenomeSeq</t>
   </si>
   <si>
-    <t>MODEL-AD_5XFAD</t>
+    <t>MODEL-AD_Abca7_APOE4_Trem2</t>
   </si>
   <si>
     <t>SiMoA</t>
   </si>
   <si>
-    <t>MODEL-AD_Abca7_APOE4_Trem2</t>
+    <t>MODEL-AD_APOE4_KI</t>
   </si>
   <si>
     <t>snATACSeq</t>
   </si>
   <si>
-    <t>MODEL-AD_APOE4_KI</t>
+    <t>MODEL-AD_APOE4_Trem2</t>
   </si>
   <si>
     <t>snpArray</t>
   </si>
   <si>
-    <t>MODEL-AD_APOE4_Trem2</t>
+    <t>MODEL-AD_Ceacam_KO_APOE4_Trem2</t>
   </si>
   <si>
     <t>snrnaSeq</t>
   </si>
   <si>
-    <t>MODEL-AD_Ceacam_KO_APOE4_Trem2</t>
+    <t>MODEL-AD_hAbeta_KI</t>
   </si>
   <si>
     <t>spontaneous alternation</t>
   </si>
   <si>
-    <t>MODEL-AD_hAbeta_KI</t>
+    <t>MODEL-AD_Harmonization</t>
   </si>
   <si>
     <t>STARRSeq</t>
   </si>
   <si>
-    <t>MODEL-AD_Harmonization</t>
+    <t>MODEL-AD_hCR1_KI_on_APOE4_Trem2</t>
   </si>
   <si>
     <t>TMT quantitation</t>
   </si>
   <si>
-    <t>MODEL-AD_hCR1_KI_on_APOE4_Trem2</t>
+    <t>MODEL-AD_hTau_Trem2</t>
   </si>
   <si>
     <t>TotalRNAseq</t>
   </si>
   <si>
-    <t>MODEL-AD_hTau_Trem2</t>
+    <t>MODEL-AD_Il1rapKO_APOE4_Trem2_exon2KO</t>
   </si>
   <si>
     <t>tractionForceMicroscopy</t>
   </si>
   <si>
-    <t>MODEL-AD_Il1rapKO_APOE4_Trem2_exon2KO</t>
+    <t>MODEL-AD_Mthfr_APOE4_Trem2</t>
   </si>
   <si>
     <t>UC Davis GCTOF</t>
   </si>
   <si>
-    <t>MODEL-AD_Mthfr_APOE4_Trem2</t>
+    <t>MODEL-AD_Rat_F344</t>
   </si>
   <si>
     <t>UCSD Untargeted Metabolomics</t>
   </si>
   <si>
-    <t>MODEL-AD_Rat_F344</t>
+    <t>MODEL-AD_Trem2_R47H</t>
   </si>
   <si>
     <t>UPLC-ESI-QTOF-MS</t>
   </si>
   <si>
-    <t>MODEL-AD_Trem2_R47H</t>
+    <t>MouseHAL</t>
   </si>
   <si>
     <t>UPLC-MSMS</t>
   </si>
   <si>
-    <t>MouseHAL</t>
+    <t>MRGWAS</t>
   </si>
   <si>
     <t>Vernier Caliper</t>
   </si>
   <si>
-    <t>MRGWAS</t>
+    <t>MSBB</t>
   </si>
   <si>
     <t>von Frey test</t>
   </si>
   <si>
-    <t>MSBB</t>
+    <t>MSBB_ArrayTissuePanel</t>
   </si>
   <si>
     <t>westernBlot</t>
   </si>
   <si>
-    <t>MSBB_ArrayTissuePanel</t>
+    <t>MSDM</t>
   </si>
   <si>
     <t>wheel running</t>
   </si>
   <si>
-    <t>MSDM</t>
+    <t>MSMM</t>
   </si>
   <si>
     <t>whole-cell patch clamp</t>
   </si>
   <si>
-    <t>MSMM</t>
+    <t>MSSMiPSC</t>
   </si>
   <si>
     <t>wholeGenomeSeq</t>
   </si>
   <si>
-    <t>MSSMiPSC</t>
+    <t>mtDNA_AD</t>
   </si>
   <si>
     <t>Wishart Catecholamines</t>
   </si>
   <si>
-    <t>mtDNA_AD</t>
+    <t>NAPS</t>
   </si>
   <si>
     <t>Wishart High Value Metabolites</t>
   </si>
   <si>
-    <t>NAPS</t>
+    <t>NHP-Chimpanzee</t>
   </si>
   <si>
     <t>Zeno Electronic Walkway</t>
   </si>
   <si>
-    <t>NHP-Chimpanzee</t>
-  </si>
-  <si>
     <t>NHP-Macaque</t>
   </si>
   <si>
@@ -1780,9 +1777,6 @@
   </si>
   <si>
     <t>UPenn</t>
-  </si>
-  <si>
-    <t>Virus_Resilience_Organoids</t>
   </si>
   <si>
     <t>VirusResilience_Banner</t>
@@ -29211,14 +29205,14 @@
       <formula>$M1 = "metadata"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1000">
+  <conditionalFormatting sqref="O1:O1000">
     <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>$K1 = "experimentalData"</formula>
+      <formula>$K1 = "analysis"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1000">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
-      <formula>$K1 = "experimentalData"</formula>
+  <conditionalFormatting sqref="N1:N1000">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+      <formula>$K1 = "metadata"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1000">
@@ -29226,19 +29220,19 @@
       <formula>$K1 = "experimentalData"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1000">
-    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="F1:F1000">
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>$K1 = "experimentalData"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1000">
+  <conditionalFormatting sqref="M1:M1000">
     <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
-      <formula>$K1 = "analysis"</formula>
+      <formula>$K1 = "experimentalData"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1000">
+  <conditionalFormatting sqref="L1:L1000">
     <cfRule type="expression" dxfId="0" priority="7" stopIfTrue="1">
-      <formula>$K1 = "metadata"</formula>
+      <formula>$K1 = "experimentalData"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
@@ -29260,9 +29254,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="O2:O1000">
       <formula1>Sheet2!$O$2:$O$49</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="I2:I1000">
-      <formula1>Sheet2!$I$2:$I$191</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="F2:F1000">
       <formula1>Sheet2!$F$2:$F$123</formula1>
     </dataValidation>
@@ -29271,6 +29262,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="L2:L1000">
       <formula1>Sheet2!$L$2:$L$24</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="I2:I1000">
+      <formula1>Sheet2!$I$2:$I$189</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="N2:N1000">
       <formula1>Sheet2!$N$2:$N$9</formula1>
@@ -31382,16 +31376,6 @@
         <v>564</v>
       </c>
     </row>
-    <row r="190">
-      <c r="I190" s="7" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="I191" s="7" t="s">
-        <v>566</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "add changed manifests"
This reverts commit 37c7858699435d32c173af1c0b86bbf2870cc215.
</commit_message>
<xml_diff>
--- a/current-excel-manifests/FileAnnotationTemplate.xlsx
+++ b/current-excel-manifests/FileAnnotationTemplate.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="565">
   <si>
     <t>Component</t>
   </si>
@@ -984,7 +984,7 @@
     <t>json</t>
   </si>
   <si>
-    <t>DivCo_HS</t>
+    <t>DukeAD_PTSD</t>
   </si>
   <si>
     <t>transcript quantification</t>
@@ -996,7 +996,7 @@
     <t>locs</t>
   </si>
   <si>
-    <t>DukeAD_PTSD</t>
+    <t>ELPSCRNA</t>
   </si>
   <si>
     <t>variancePartition</t>
@@ -1008,7 +1008,7 @@
     <t>maf</t>
   </si>
   <si>
-    <t>ELPSCRNA</t>
+    <t>Emory_ADRC</t>
   </si>
   <si>
     <t>Variant calling</t>
@@ -1020,7 +1020,7 @@
     <t>mat</t>
   </si>
   <si>
-    <t>Emory_ADRC</t>
+    <t>Emory_Levey_300_CSF_FNIH</t>
   </si>
   <si>
     <t>visualization</t>
@@ -1032,7 +1032,7 @@
     <t>md</t>
   </si>
   <si>
-    <t>Emory_Levey_300_CSF_FNIH</t>
+    <t>EmoryDrosophilaTau</t>
   </si>
   <si>
     <t>LC-SRM</t>
@@ -1041,7 +1041,7 @@
     <t>mov</t>
   </si>
   <si>
-    <t>EmoryDrosophilaTau</t>
+    <t>EpiGABA</t>
   </si>
   <si>
     <t>Leiden Oxylipins</t>
@@ -1050,7 +1050,7 @@
     <t>mp4</t>
   </si>
   <si>
-    <t>EpiGABA</t>
+    <t>EpiMap</t>
   </si>
   <si>
     <t>lentiMPRA</t>
@@ -1059,7 +1059,7 @@
     <t>msf</t>
   </si>
   <si>
-    <t>EpiMap</t>
+    <t>eQTLmetaAnalysis</t>
   </si>
   <si>
     <t>LFP</t>
@@ -1068,7 +1068,7 @@
     <t>mtx</t>
   </si>
   <si>
-    <t>eQTLmetaAnalysis</t>
+    <t>FreshMicro</t>
   </si>
   <si>
     <t>liquid chromatography-electrochemical detection</t>
@@ -1077,7 +1077,7 @@
     <t>nirs</t>
   </si>
   <si>
-    <t>FreshMicro</t>
+    <t>HBI_scRNAseq</t>
   </si>
   <si>
     <t>lncrnaSeq</t>
@@ -1086,7 +1086,7 @@
     <t>pdf</t>
   </si>
   <si>
-    <t>HBI_scRNAseq</t>
+    <t>HBTRC</t>
   </si>
   <si>
     <t>locomotor activation behavior</t>
@@ -1095,7 +1095,7 @@
     <t>pdresult</t>
   </si>
   <si>
-    <t>HBTRC</t>
+    <t>HDAC1-cKOBrain</t>
   </si>
   <si>
     <t>long-read rnaSeq</t>
@@ -1104,7 +1104,7 @@
     <t>pdstudy</t>
   </si>
   <si>
-    <t>HDAC1-cKOBrain</t>
+    <t>HumanFC</t>
   </si>
   <si>
     <t>LTP</t>
@@ -1113,7 +1113,7 @@
     <t>pdview</t>
   </si>
   <si>
-    <t>HumanFC</t>
+    <t>IL10_APPmouse</t>
   </si>
   <si>
     <t>m6A-rnaSeq</t>
@@ -1122,7 +1122,7 @@
     <t>plink</t>
   </si>
   <si>
-    <t>IL10_APPmouse</t>
+    <t>iNiAstshRNA</t>
   </si>
   <si>
     <t>MDMS-SL</t>
@@ -1131,7 +1131,7 @@
     <t>png</t>
   </si>
   <si>
-    <t>iNiAstshRNA</t>
+    <t>IntegrativePathwayAnalysis</t>
   </si>
   <si>
     <t>memory behavior</t>
@@ -1140,7 +1140,7 @@
     <t>powerpoint</t>
   </si>
   <si>
-    <t>IntegrativePathwayAnalysis</t>
+    <t>iPSC</t>
   </si>
   <si>
     <t>Metabolon</t>
@@ -1149,7 +1149,7 @@
     <t>Python script</t>
   </si>
   <si>
-    <t>iPSC</t>
+    <t>iPSC-HiC</t>
   </si>
   <si>
     <t>methylationArray</t>
@@ -1158,7 +1158,7 @@
     <t>pzfx</t>
   </si>
   <si>
-    <t>iPSC-HiC</t>
+    <t>iPSCAstrocytes</t>
   </si>
   <si>
     <t>MIB/MS</t>
@@ -1167,13 +1167,13 @@
     <t>R script</t>
   </si>
   <si>
-    <t>iPSCAstrocytes</t>
+    <t>iPSCMicroglia</t>
   </si>
   <si>
     <t>microRNAcounts</t>
   </si>
   <si>
-    <t>iPSCMicroglia</t>
+    <t>ISB_Taner_CollagenDomain</t>
   </si>
   <si>
     <t>mirnaArray</t>
@@ -1182,7 +1182,7 @@
     <t>RCC</t>
   </si>
   <si>
-    <t>ISB_Taner_CollagenDomain</t>
+    <t>ISB_Taner_Cxcl10</t>
   </si>
   <si>
     <t>mirnaSeq</t>
@@ -1191,7 +1191,7 @@
     <t>RData</t>
   </si>
   <si>
-    <t>ISB_Taner_Cxcl10</t>
+    <t>ISB_Taner_PTN_MDK</t>
   </si>
   <si>
     <t>MRI</t>
@@ -1200,7 +1200,7 @@
     <t>recal</t>
   </si>
   <si>
-    <t>ISB_Taner_PTN_MDK</t>
+    <t>ISB_Taner_sIL10r_sIL4r</t>
   </si>
   <si>
     <t>mRNAcounts</t>
@@ -1209,7 +1209,7 @@
     <t>RLF</t>
   </si>
   <si>
-    <t>ISB_Taner_sIL10r_sIL4r</t>
+    <t>ISB_Taner_TGFbeta</t>
   </si>
   <si>
     <t>mRNAseq</t>
@@ -1218,7 +1218,7 @@
     <t>rmd</t>
   </si>
   <si>
-    <t>ISB_Taner_TGFbeta</t>
+    <t>Jax.IU.Pitt.Proteomics_Metabolomics_Pilot</t>
   </si>
   <si>
     <t>MudPIT</t>
@@ -1227,7 +1227,7 @@
     <t>saf</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt.Proteomics_Metabolomics_Pilot</t>
+    <t>Jax.IU.Pitt_APOE4.Trem2.R47H</t>
   </si>
   <si>
     <t>nextGenerationTargetedSequencing</t>
@@ -1236,7 +1236,7 @@
     <t>sam</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_APOE4.Trem2.R47H</t>
+    <t>Jax.IU.Pitt_APP.PS1</t>
   </si>
   <si>
     <t>Nightingale NMR</t>
@@ -1245,7 +1245,7 @@
     <t>sav</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_APP.PS1</t>
+    <t>Jax.IU.Pitt_Levetiracetam-5XFAD</t>
   </si>
   <si>
     <t>NOMe-Seq</t>
@@ -1254,7 +1254,7 @@
     <t>sdf</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_Levetiracetam-5XFAD</t>
+    <t>Jax.IU.Pitt_LOAD2.PrimaryScreen</t>
   </si>
   <si>
     <t>novelty response behavior</t>
@@ -1263,7 +1263,7 @@
     <t>seg</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_LOAD2.PrimaryScreen</t>
+    <t>Jax.IU.Pitt_MicrobiomePilot</t>
   </si>
   <si>
     <t>open field test</t>
@@ -1272,7 +1272,7 @@
     <t>Sentrix descriptor file</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_MicrobiomePilot</t>
+    <t>Jax.IU.Pitt_PrimaryScreen</t>
   </si>
   <si>
     <t>oxBS-Seq</t>
@@ -1281,7 +1281,7 @@
     <t>sf3</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_PrimaryScreen</t>
+    <t>Jax.IU.Pitt_StrainValidation</t>
   </si>
   <si>
     <t>pharmacodynamics</t>
@@ -1290,7 +1290,7 @@
     <t>sif</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_StrainValidation</t>
+    <t>Jax.IU.Pitt_Verubecestat_5XFAD</t>
   </si>
   <si>
     <t>pharmacokinetics</t>
@@ -1299,7 +1299,7 @@
     <t>sqlite</t>
   </si>
   <si>
-    <t>Jax.IU.Pitt_Verubecestat_5XFAD</t>
+    <t>LBP</t>
   </si>
   <si>
     <t>photograph</t>
@@ -1308,7 +1308,7 @@
     <t>sra</t>
   </si>
   <si>
-    <t>LBP</t>
+    <t>LillyMicroglia</t>
   </si>
   <si>
     <t>polymeraseChainReaction</t>
@@ -1317,7 +1317,7 @@
     <t>svg</t>
   </si>
   <si>
-    <t>LillyMicroglia</t>
+    <t>LLFS</t>
   </si>
   <si>
     <t>Positron Emission Tomography</t>
@@ -1326,7 +1326,7 @@
     <t>svs</t>
   </si>
   <si>
-    <t>LLFS</t>
+    <t>lncRNA Pilot</t>
   </si>
   <si>
     <t>proximity extension assay</t>
@@ -1335,7 +1335,7 @@
     <t>Synapse Table</t>
   </si>
   <si>
-    <t>lncRNA Pilot</t>
+    <t>MARS WISCONSIN</t>
   </si>
   <si>
     <t>questionnaire</t>
@@ -1344,7 +1344,7 @@
     <t>tab</t>
   </si>
   <si>
-    <t>MARS WISCONSIN</t>
+    <t>MayoeGWAS</t>
   </si>
   <si>
     <t>Rader Lipidomics</t>
@@ -1353,7 +1353,7 @@
     <t>tagAlign</t>
   </si>
   <si>
-    <t>MayoeGWAS</t>
+    <t>MayoHippocampus</t>
   </si>
   <si>
     <t>Real Time PCR</t>
@@ -1362,7 +1362,7 @@
     <t>tar</t>
   </si>
   <si>
-    <t>MayoHippocampus</t>
+    <t>MayoLOADGWAS</t>
   </si>
   <si>
     <t>Ribo-Seq</t>
@@ -1371,7 +1371,7 @@
     <t>tbi</t>
   </si>
   <si>
-    <t>MayoLOADGWAS</t>
+    <t>MayoPilotRNAseq</t>
   </si>
   <si>
     <t>rnaArray</t>
@@ -1380,7 +1380,7 @@
     <t>tif</t>
   </si>
   <si>
-    <t>MayoPilotRNAseq</t>
+    <t>MayoRNAseq</t>
   </si>
   <si>
     <t>rnaSeq</t>
@@ -1389,7 +1389,7 @@
     <t>tranches</t>
   </si>
   <si>
-    <t>MayoRNAseq</t>
+    <t>MC-BrAD</t>
   </si>
   <si>
     <t>rotarod performance test</t>
@@ -1398,7 +1398,7 @@
     <t>tsv</t>
   </si>
   <si>
-    <t>MC-BrAD</t>
+    <t>MC-CAA</t>
   </si>
   <si>
     <t>RPPA</t>
@@ -1407,7 +1407,7 @@
     <t>txt</t>
   </si>
   <si>
-    <t>MC-CAA</t>
+    <t>MC_snRNA</t>
   </si>
   <si>
     <t>RRBS</t>
@@ -1416,7 +1416,7 @@
     <t>vcf</t>
   </si>
   <si>
-    <t>MC_snRNA</t>
+    <t>mCITE-Seq</t>
   </si>
   <si>
     <t>sandwich ELISA</t>
@@ -1425,7 +1425,7 @@
     <t>wiggle</t>
   </si>
   <si>
-    <t>mCITE-Seq</t>
+    <t>MCMPS</t>
   </si>
   <si>
     <t>Sanger sequencing</t>
@@ -1434,7 +1434,7 @@
     <t>xml</t>
   </si>
   <si>
-    <t>MCMPS</t>
+    <t>MEF2_Resilience</t>
   </si>
   <si>
     <t>scale</t>
@@ -1443,7 +1443,7 @@
     <t>yaml</t>
   </si>
   <si>
-    <t>MEF2_Resilience</t>
+    <t>MindPhenomeKB</t>
   </si>
   <si>
     <t>scATACSeq</t>
@@ -1452,165 +1452,162 @@
     <t>zip</t>
   </si>
   <si>
-    <t>MindPhenomeKB</t>
+    <t>miR155</t>
   </si>
   <si>
     <t>scCGIseq</t>
   </si>
   <si>
-    <t>miR155</t>
+    <t>MIT_ROSMAP_Multiomics</t>
   </si>
   <si>
     <t>scirnaSeq</t>
   </si>
   <si>
-    <t>MIT_ROSMAP_Multiomics</t>
+    <t>MOA-PAD</t>
   </si>
   <si>
     <t>scrnaSeq</t>
   </si>
   <si>
-    <t>MOA-PAD</t>
+    <t>MODEL-AD_5XFAD</t>
   </si>
   <si>
     <t>scwholeGenomeSeq</t>
   </si>
   <si>
-    <t>MODEL-AD_5XFAD</t>
+    <t>MODEL-AD_Abca7_APOE4_Trem2</t>
   </si>
   <si>
     <t>SiMoA</t>
   </si>
   <si>
-    <t>MODEL-AD_Abca7_APOE4_Trem2</t>
+    <t>MODEL-AD_APOE4_KI</t>
   </si>
   <si>
     <t>snATACSeq</t>
   </si>
   <si>
-    <t>MODEL-AD_APOE4_KI</t>
+    <t>MODEL-AD_APOE4_Trem2</t>
   </si>
   <si>
     <t>snpArray</t>
   </si>
   <si>
-    <t>MODEL-AD_APOE4_Trem2</t>
+    <t>MODEL-AD_Ceacam_KO_APOE4_Trem2</t>
   </si>
   <si>
     <t>snrnaSeq</t>
   </si>
   <si>
-    <t>MODEL-AD_Ceacam_KO_APOE4_Trem2</t>
+    <t>MODEL-AD_hAbeta_KI</t>
   </si>
   <si>
     <t>spontaneous alternation</t>
   </si>
   <si>
-    <t>MODEL-AD_hAbeta_KI</t>
+    <t>MODEL-AD_Harmonization</t>
   </si>
   <si>
     <t>STARRSeq</t>
   </si>
   <si>
-    <t>MODEL-AD_Harmonization</t>
+    <t>MODEL-AD_hCR1_KI_on_APOE4_Trem2</t>
   </si>
   <si>
     <t>TMT quantitation</t>
   </si>
   <si>
-    <t>MODEL-AD_hCR1_KI_on_APOE4_Trem2</t>
+    <t>MODEL-AD_hTau_Trem2</t>
   </si>
   <si>
     <t>TotalRNAseq</t>
   </si>
   <si>
-    <t>MODEL-AD_hTau_Trem2</t>
+    <t>MODEL-AD_Il1rapKO_APOE4_Trem2_exon2KO</t>
   </si>
   <si>
     <t>tractionForceMicroscopy</t>
   </si>
   <si>
-    <t>MODEL-AD_Il1rapKO_APOE4_Trem2_exon2KO</t>
+    <t>MODEL-AD_Mthfr_APOE4_Trem2</t>
   </si>
   <si>
     <t>UC Davis GCTOF</t>
   </si>
   <si>
-    <t>MODEL-AD_Mthfr_APOE4_Trem2</t>
+    <t>MODEL-AD_Rat_F344</t>
   </si>
   <si>
     <t>UCSD Untargeted Metabolomics</t>
   </si>
   <si>
-    <t>MODEL-AD_Rat_F344</t>
+    <t>MODEL-AD_Trem2_R47H</t>
   </si>
   <si>
     <t>UPLC-ESI-QTOF-MS</t>
   </si>
   <si>
-    <t>MODEL-AD_Trem2_R47H</t>
+    <t>MouseHAL</t>
   </si>
   <si>
     <t>UPLC-MSMS</t>
   </si>
   <si>
-    <t>MouseHAL</t>
+    <t>MRGWAS</t>
   </si>
   <si>
     <t>Vernier Caliper</t>
   </si>
   <si>
-    <t>MRGWAS</t>
+    <t>MSBB</t>
   </si>
   <si>
     <t>von Frey test</t>
   </si>
   <si>
-    <t>MSBB</t>
+    <t>MSBB_ArrayTissuePanel</t>
   </si>
   <si>
     <t>westernBlot</t>
   </si>
   <si>
-    <t>MSBB_ArrayTissuePanel</t>
+    <t>MSDM</t>
   </si>
   <si>
     <t>wheel running</t>
   </si>
   <si>
-    <t>MSDM</t>
+    <t>MSMM</t>
   </si>
   <si>
     <t>whole-cell patch clamp</t>
   </si>
   <si>
-    <t>MSMM</t>
+    <t>MSSMiPSC</t>
   </si>
   <si>
     <t>wholeGenomeSeq</t>
   </si>
   <si>
-    <t>MSSMiPSC</t>
+    <t>mtDNA_AD</t>
   </si>
   <si>
     <t>Wishart Catecholamines</t>
   </si>
   <si>
-    <t>mtDNA_AD</t>
+    <t>NAPS</t>
   </si>
   <si>
     <t>Wishart High Value Metabolites</t>
   </si>
   <si>
-    <t>NAPS</t>
+    <t>NHP-Chimpanzee</t>
   </si>
   <si>
     <t>Zeno Electronic Walkway</t>
   </si>
   <si>
-    <t>NHP-Chimpanzee</t>
-  </si>
-  <si>
     <t>NHP-Macaque</t>
   </si>
   <si>
@@ -1780,9 +1777,6 @@
   </si>
   <si>
     <t>UPenn</t>
-  </si>
-  <si>
-    <t>Virus_Resilience_Organoids</t>
   </si>
   <si>
     <t>VirusResilience_Banner</t>
@@ -29211,34 +29205,34 @@
       <formula>$M1 = "metadata"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1000">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>$K1 = "analysis"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:N1000">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+      <formula>$K1 = "metadata"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1000">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>$K1 = "experimentalData"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1000">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>$K1 = "experimentalData"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1000">
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
       <formula>$K1 = "experimentalData"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1000">
-    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="7" stopIfTrue="1">
       <formula>$K1 = "experimentalData"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1000">
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
-      <formula>$K1 = "analysis"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1000">
-    <cfRule type="expression" dxfId="0" priority="7" stopIfTrue="1">
-      <formula>$K1 = "metadata"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
@@ -29260,9 +29254,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="O2:O1000">
       <formula1>Sheet2!$O$2:$O$49</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="I2:I1000">
-      <formula1>Sheet2!$I$2:$I$191</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="F2:F1000">
       <formula1>Sheet2!$F$2:$F$123</formula1>
     </dataValidation>
@@ -29271,6 +29262,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="L2:L1000">
       <formula1>Sheet2!$L$2:$L$24</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="I2:I1000">
+      <formula1>Sheet2!$I$2:$I$189</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="N2:N1000">
       <formula1>Sheet2!$N$2:$N$9</formula1>
@@ -31382,16 +31376,6 @@
         <v>564</v>
       </c>
     </row>
-    <row r="190">
-      <c r="I190" s="7" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="I191" s="7" t="s">
-        <v>566</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>